<commit_message>
Capacitor Kit 603 is added
</commit_message>
<xml_diff>
--- a/Facilities/Machinery-Lab/passive-components/smd-capacitor-set/Capacitor-Kit.xlsx
+++ b/Facilities/Machinery-Lab/passive-components/smd-capacitor-set/Capacitor-Kit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="BuÇalismaKitabi" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozgur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macit\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C0FE0A-3A48-4B6D-B0DA-7852B21CDD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256267B4-987D-463E-8E79-6CE8B939E511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3B855C3-EF76-4A1A-A70B-1495EC5141DB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3B855C3-EF76-4A1A-A70B-1495EC5141DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="137">
   <si>
     <t>E12 Series Capacitor Selection [2024-02-23]</t>
   </si>
@@ -253,6 +253,201 @@
   </si>
   <si>
     <t>CL05B152KB5VPNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C010BB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C1R2BB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C1R5CB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C1R8CB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : MCF03CTN5002R2</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : MCF03CTN5003R3</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603CRNPO9BN3R9</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C4R7BB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603CRNPO9BN5R6</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603CRNPO9BN6R8</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C100JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C120JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPO9BN150</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C180JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPO9BN220</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C270JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPO9BN330</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPO9BN390</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C470JC8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPOABN560</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C680JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C820JB81PND</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C910JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPO9BN101</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C121JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPO9BN151</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C221JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPOYBN271</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C331JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B391KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603JRNPO9BN471</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C511JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C561JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10C681JB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B102KC8NNND</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603KRX7R9BB122</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603KRX7R9BB152</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B182KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B222KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603KRX7R0BB332</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B392KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B472KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B562KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B682KB8WPNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B822KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B153KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B223KA8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B273KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B333KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603KRX7R9BB393</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B473KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B563KA8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B683KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B823KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B154KA8VPNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B224KB8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : C0603274K1CBT</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : BX0603334K1ENR</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B474KA8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CC0603KRX7R7BB684</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10B105KA8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : CL10A225KO8NNNC</t>
+  </si>
+  <si>
+    <t>Ürün Kodu : MCF03MTX250106</t>
   </si>
 </sst>
 </file>
@@ -260,11 +455,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="167" formatCode="#,##0.0\ &quot;pF&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0\ &quot;pF&quot;"/>
-    <numFmt numFmtId="169" formatCode="#,##0,\ &quot;nF&quot;"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0,\ &quot;nF&quot;"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0,,\ &quot;µF&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;pF&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0\ &quot;pF&quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0,\ &quot;nF&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0,\ &quot;nF&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0,,\ &quot;µF&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -326,26 +521,26 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -662,35 +857,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA03285-25F9-4A01-A5EF-42DD42588C1B}">
   <sheetPr codeName="Sayfa2"/>
-  <dimension ref="A1:V99"/>
+  <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -700,19 +885,11 @@
       <c r="C2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D2" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1.2</v>
       </c>
@@ -722,19 +899,11 @@
       <c r="C3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D3" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1.5</v>
       </c>
@@ -744,20 +913,18 @@
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D4" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="18"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.8</v>
       </c>
@@ -767,19 +934,18 @@
       <c r="C5" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="18"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -789,20 +955,18 @@
       <c r="C6" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D6" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="14"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="18"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2.7</v>
       </c>
@@ -812,19 +976,16 @@
       <c r="C7" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D7" s="12"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="18"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3.3</v>
       </c>
@@ -834,37 +995,34 @@
       <c r="C8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D8" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="18"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>3.9</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D9" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" s="14"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="18"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>4.7</v>
       </c>
@@ -874,19 +1032,18 @@
       <c r="C10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D10" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" s="14"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="18"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>5.0999999999999996</v>
       </c>
@@ -896,36 +1053,32 @@
       <c r="C11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D11" s="12"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="18"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>5.6</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" s="14"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="18"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>6.8</v>
       </c>
@@ -935,19 +1088,18 @@
       <c r="C13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D13" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" s="14"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="18"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>8.1999999999999993</v>
       </c>
@@ -957,36 +1109,28 @@
       <c r="C14" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D14" s="12"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="18"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>9.1</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N15" s="14"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="18"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f t="shared" ref="A16:A47" si="0">A2*10</f>
         <v>10</v>
@@ -997,19 +1141,18 @@
       <c r="C16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D16" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="14"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="18"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1020,19 +1163,18 @@
       <c r="C17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D17" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="N17" s="14"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="18"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1043,20 +1185,11 @@
       <c r="C18" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D18" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1067,20 +1200,11 @@
       <c r="C19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D19" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1091,8 +1215,11 @@
       <c r="C20" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D20" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1103,9 +1230,11 @@
       <c r="C21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D21" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1116,9 +1245,11 @@
       <c r="C22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D22" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1129,8 +1260,11 @@
       <c r="C23" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D23" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1141,8 +1275,11 @@
       <c r="C24" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D24" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1153,8 +1290,9 @@
       <c r="C25" s="12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1165,9 +1303,11 @@
       <c r="C26" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D26" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -1178,22 +1318,30 @@
       <c r="C27" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D27" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="C28" s="13"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D28" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D29" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -1204,8 +1352,11 @@
       <c r="C30" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D30" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>120</v>
@@ -1216,9 +1367,11 @@
       <c r="C31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D31" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>150</v>
@@ -1229,6 +1382,9 @@
       <c r="C32" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="D32" s="19" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
@@ -1241,6 +1397,7 @@
       <c r="C33" s="12" t="s">
         <v>50</v>
       </c>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
@@ -1253,7 +1410,9 @@
       <c r="C34" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="13"/>
+      <c r="D34" s="19" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
@@ -1266,7 +1425,9 @@
       <c r="C35" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="13"/>
+      <c r="D35" s="19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
@@ -1279,6 +1440,9 @@
       <c r="C36" s="12" t="s">
         <v>53</v>
       </c>
+      <c r="D36" s="19" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
@@ -1286,6 +1450,9 @@
         <v>390</v>
       </c>
       <c r="C37" s="13"/>
+      <c r="D37" s="19" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
@@ -1298,12 +1465,18 @@
       <c r="C38" s="12" t="s">
         <v>59</v>
       </c>
+      <c r="D38" s="19" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>510</v>
       </c>
+      <c r="D39" s="19" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
@@ -1316,7 +1489,9 @@
       <c r="C40" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="13"/>
+      <c r="D40" s="19" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
@@ -1329,6 +1504,9 @@
       <c r="C41" s="12" t="s">
         <v>66</v>
       </c>
+      <c r="D41" s="19" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
@@ -1341,6 +1519,7 @@
       <c r="C42" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -1348,6 +1527,7 @@
         <v>910</v>
       </c>
       <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
@@ -1360,6 +1540,9 @@
       <c r="C44" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="D44" s="19" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
@@ -1372,7 +1555,9 @@
       <c r="C45" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="13"/>
+      <c r="D45" s="19" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
@@ -1385,11 +1570,17 @@
       <c r="C46" s="12" t="s">
         <v>71</v>
       </c>
+      <c r="D46" s="19" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <f t="shared" si="0"/>
         <v>1800</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1403,6 +1594,9 @@
       <c r="C48" s="12" t="s">
         <v>62</v>
       </c>
+      <c r="D48" s="19" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
@@ -1410,6 +1604,7 @@
         <v>2700</v>
       </c>
       <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
@@ -1422,6 +1617,9 @@
       <c r="C50" s="12" t="s">
         <v>61</v>
       </c>
+      <c r="D50" s="19" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
@@ -1434,7 +1632,9 @@
       <c r="C51" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="13"/>
+      <c r="D51" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
@@ -1447,7 +1647,9 @@
       <c r="C52" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="13"/>
+      <c r="D52" s="19" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
@@ -1455,12 +1657,16 @@
         <v>5100</v>
       </c>
       <c r="C53" s="13"/>
+      <c r="D53" s="19"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <f t="shared" si="1"/>
         <v>5600</v>
       </c>
+      <c r="D54" s="19" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
@@ -1473,6 +1679,9 @@
       <c r="C55" s="12" t="s">
         <v>36</v>
       </c>
+      <c r="D55" s="19" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
@@ -1485,6 +1694,9 @@
       <c r="C56" s="12" t="s">
         <v>64</v>
       </c>
+      <c r="D56" s="19" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
@@ -1492,6 +1704,7 @@
         <v>9100</v>
       </c>
       <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
@@ -1504,6 +1717,9 @@
       <c r="C58" s="12" t="s">
         <v>42</v>
       </c>
+      <c r="D58" s="19" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
@@ -1511,6 +1727,7 @@
         <v>12000</v>
       </c>
       <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
@@ -1523,6 +1740,9 @@
       <c r="C60" s="12" t="s">
         <v>25</v>
       </c>
+      <c r="D60" s="19" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
@@ -1530,6 +1750,7 @@
         <v>18000</v>
       </c>
       <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
@@ -1542,6 +1763,9 @@
       <c r="C62" s="12" t="s">
         <v>56</v>
       </c>
+      <c r="D62" s="19" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
@@ -1554,6 +1778,9 @@
       <c r="C63" s="12" t="s">
         <v>70</v>
       </c>
+      <c r="D63" s="19" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
@@ -1566,16 +1793,21 @@
       <c r="C64" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D64" s="13"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <f t="shared" si="1"/>
         <v>39000</v>
       </c>
       <c r="C65" s="13"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <f t="shared" si="1"/>
         <v>47000</v>
@@ -1586,21 +1818,28 @@
       <c r="C66" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <f t="shared" si="1"/>
         <v>51000</v>
       </c>
       <c r="C67" s="13"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="13"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <f t="shared" si="1"/>
         <v>56000</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <f t="shared" si="1"/>
         <v>68000</v>
@@ -1611,8 +1850,11 @@
       <c r="C69" s="12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <f t="shared" si="1"/>
         <v>82000</v>
@@ -1623,15 +1865,19 @@
       <c r="C70" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <f t="shared" si="1"/>
         <v>91000</v>
       </c>
       <c r="C71" s="13"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="13"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <f t="shared" si="1"/>
         <v>100000</v>
@@ -1642,69 +1888,88 @@
       <c r="C72" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <f t="shared" si="1"/>
         <v>120000</v>
       </c>
       <c r="C73" s="13"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="19"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <f t="shared" si="1"/>
         <v>150000</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <f t="shared" si="1"/>
         <v>180000</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <f t="shared" si="1"/>
         <v>220000</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <f t="shared" si="1"/>
         <v>270000</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <f t="shared" si="1"/>
         <v>330000</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <f t="shared" si="1"/>
         <v>390000</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <f t="shared" ref="A80:A99" si="2">A66*10</f>
         <v>470000</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <f t="shared" si="2"/>
         <v>510000</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <f t="shared" si="2"/>
         <v>560000</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <f t="shared" si="2"/>
         <v>680000</v>
@@ -1715,21 +1980,25 @@
       <c r="C83" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <f t="shared" si="2"/>
         <v>820000</v>
       </c>
       <c r="C84" s="13"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="13"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <f t="shared" si="2"/>
         <v>910000</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="10">
         <f t="shared" si="2"/>
         <v>1000000</v>
@@ -1740,27 +2009,31 @@
       <c r="C86" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
         <f t="shared" si="2"/>
         <v>1200000</v>
       </c>
       <c r="C87" s="13"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="13"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="10">
         <f t="shared" si="2"/>
         <v>1500000</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
         <f t="shared" si="2"/>
         <v>1800000</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="10">
         <f t="shared" si="2"/>
         <v>2200000</v>
@@ -1771,27 +2044,31 @@
       <c r="C90" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="10">
         <f t="shared" si="2"/>
         <v>2700000</v>
       </c>
       <c r="C91" s="13"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="13"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="10">
         <f t="shared" si="2"/>
         <v>3300000</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="10">
         <f t="shared" si="2"/>
         <v>3900000</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="10">
         <f t="shared" si="2"/>
         <v>4700000</v>
@@ -1802,36 +2079,58 @@
       <c r="C94" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <f t="shared" si="2"/>
         <v>5100000</v>
       </c>
       <c r="C95" s="13"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="10">
         <f t="shared" si="2"/>
         <v>5600000</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
         <f t="shared" si="2"/>
         <v>6800000</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="10">
         <f t="shared" si="2"/>
         <v>8200000</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
-        <f t="shared" si="2"/>
+        <f>A85*10</f>
         <v>9100000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="11">
+        <f>A86*10</f>
+        <v>10000000</v>
+      </c>
+      <c r="D100" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <f>COUNTA(C2:C101)</f>
+        <v>56</v>
+      </c>
+      <c r="D102">
+        <f>COUNTA(D2:D101)</f>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1892,6 +2191,72 @@
     <hyperlink ref="C3" r:id="rId54" display="https://ozdisan.com/Product/Detail/957147" xr:uid="{C8A2C3A9-8927-491D-BEF7-88E6CDAF700B}"/>
     <hyperlink ref="C63" r:id="rId55" display="https://ozdisan.com/Product/Detail/521939" xr:uid="{8BF067B3-FA62-49A9-9CA2-0FD2384DB265}"/>
     <hyperlink ref="C46" r:id="rId56" display="https://ozdisan.com/pasif-komponentler/kapasitorler/smt-smd-ve-mlcc-kapasitorler/CL05B152KB5VPNC/521919" xr:uid="{17BCC61C-093E-4ABF-BD4B-BC98DDD29472}"/>
+    <hyperlink ref="D2" r:id="rId57" xr:uid="{013E6BC3-080E-42C6-A2C9-4C6C2D546EDC}"/>
+    <hyperlink ref="D3" r:id="rId58" xr:uid="{26AA1B37-52D8-4D40-AE07-573F2E47C3CB}"/>
+    <hyperlink ref="D4" r:id="rId59" xr:uid="{BD4B6F20-6929-4F47-956B-57D756C6FCDE}"/>
+    <hyperlink ref="D5" r:id="rId60" xr:uid="{B9339B8C-5EAF-40F8-8009-E0461DDD4FA5}"/>
+    <hyperlink ref="D6" r:id="rId61" xr:uid="{0FEEA4E0-F69E-4D92-A87F-0A5A1A56C071}"/>
+    <hyperlink ref="D8" r:id="rId62" xr:uid="{65470D9F-C615-40D7-8614-B74D1B3BE0BE}"/>
+    <hyperlink ref="D9" r:id="rId63" xr:uid="{E2EC6460-ADEB-4D7A-B5F8-3358201FF468}"/>
+    <hyperlink ref="D10" r:id="rId64" xr:uid="{FDE3E4D9-0BA6-4FD6-87D8-0CFEA7E8041C}"/>
+    <hyperlink ref="D12" r:id="rId65" xr:uid="{370E6946-E3EC-4D61-854C-AE2C3491545F}"/>
+    <hyperlink ref="D13" r:id="rId66" xr:uid="{7B163290-EF8F-44B7-99E8-DFAF4ED0D60E}"/>
+    <hyperlink ref="D16" r:id="rId67" xr:uid="{E6BE92C7-1E47-4B55-AFC8-1D8709E113FA}"/>
+    <hyperlink ref="D17" r:id="rId68" xr:uid="{96DFF984-D935-4CD5-B599-27A21C6E49C8}"/>
+    <hyperlink ref="D18" r:id="rId69" xr:uid="{8ED82769-E71B-4E55-B74F-64F3B511D566}"/>
+    <hyperlink ref="D19" r:id="rId70" xr:uid="{BB6C2DB2-0B1F-4C06-AF41-4EAD5DEDC463}"/>
+    <hyperlink ref="D20" r:id="rId71" xr:uid="{6F2326CF-4353-4F0A-B4B5-F4E11F183F94}"/>
+    <hyperlink ref="D21" r:id="rId72" xr:uid="{04714D8F-07ED-41C0-B970-48D1201F77B5}"/>
+    <hyperlink ref="D22" r:id="rId73" xr:uid="{9503C4E3-6A2B-4772-8FC5-B8B67ACA47DE}"/>
+    <hyperlink ref="D23" r:id="rId74" xr:uid="{78239697-5B78-40B8-A6E7-70DB907CF92A}"/>
+    <hyperlink ref="D24" r:id="rId75" xr:uid="{14400E44-BCF2-40A0-85C6-639D919EA863}"/>
+    <hyperlink ref="D26" r:id="rId76" xr:uid="{2246A5B1-1A61-4941-A4E6-84269379253E}"/>
+    <hyperlink ref="D27" r:id="rId77" xr:uid="{4A644A9C-0F65-4EBB-926E-F0B98EF093B5}"/>
+    <hyperlink ref="D28" r:id="rId78" xr:uid="{F20817BD-ECBD-422E-9316-24C7B5E2C27A}"/>
+    <hyperlink ref="D29" r:id="rId79" xr:uid="{A32DA3C2-E922-4A1C-8CA7-F2F55168D821}"/>
+    <hyperlink ref="D30" r:id="rId80" xr:uid="{FFD53D7A-7F4C-488E-88DC-12DFA928EE43}"/>
+    <hyperlink ref="D31" r:id="rId81" xr:uid="{8C1B2B28-9DC1-41AB-9B40-2B04F2C34951}"/>
+    <hyperlink ref="D32" r:id="rId82" xr:uid="{B3FE18F3-689B-49F5-B9B3-0B86591CEA3C}"/>
+    <hyperlink ref="D34" r:id="rId83" xr:uid="{300599DB-0078-4375-A0AC-456253F47384}"/>
+    <hyperlink ref="D35" r:id="rId84" xr:uid="{8A8E0CDA-E4B5-4384-98AB-37E17F1AAFB7}"/>
+    <hyperlink ref="D36" r:id="rId85" xr:uid="{B310BECB-D911-48E8-9590-A33E49B8471D}"/>
+    <hyperlink ref="D37" r:id="rId86" xr:uid="{F86E0B0F-4A31-48CC-A888-FF989E17BA4C}"/>
+    <hyperlink ref="D38" r:id="rId87" xr:uid="{2CB60A01-DF07-4665-A670-08BDEFF7205E}"/>
+    <hyperlink ref="D39" r:id="rId88" xr:uid="{35217E71-58DC-49A3-A249-4ED0341E9644}"/>
+    <hyperlink ref="D40" r:id="rId89" xr:uid="{FE56DAC2-DD51-42AF-BCD4-7F9F9C8D6A42}"/>
+    <hyperlink ref="D41" r:id="rId90" xr:uid="{C7B4E2EF-A73F-481D-9BB1-E7A6E5030906}"/>
+    <hyperlink ref="D44" r:id="rId91" xr:uid="{0CAD63B4-6F4F-493C-9E20-9B9828B96FEF}"/>
+    <hyperlink ref="D45" r:id="rId92" xr:uid="{AC7BBEF1-C0C8-4A0D-B682-B5DA1301665D}"/>
+    <hyperlink ref="D46" r:id="rId93" xr:uid="{F8031593-3BFF-4AF0-94F8-600B85160CEE}"/>
+    <hyperlink ref="D47" r:id="rId94" xr:uid="{A48A3B5A-41C5-4197-A264-267E80AD369C}"/>
+    <hyperlink ref="D48" r:id="rId95" xr:uid="{304BFCC4-8091-4F21-B36F-47D695048C12}"/>
+    <hyperlink ref="D50" r:id="rId96" xr:uid="{B2FE3831-607E-467F-AD92-4378E0444BC3}"/>
+    <hyperlink ref="D51" r:id="rId97" xr:uid="{83D08E6D-4C1A-450C-A280-503FE4839C22}"/>
+    <hyperlink ref="D52" r:id="rId98" xr:uid="{3A2AEE7F-D8A5-4050-8102-9B4E39847DB7}"/>
+    <hyperlink ref="D54" r:id="rId99" xr:uid="{4E508A7E-14B1-44C8-ABEC-27B6FBD3A977}"/>
+    <hyperlink ref="D55" r:id="rId100" xr:uid="{8A954D4F-014F-41DC-978B-DEAED1757510}"/>
+    <hyperlink ref="D56" r:id="rId101" xr:uid="{AD2FC214-BA84-4AA3-A188-FD1A79E77DAE}"/>
+    <hyperlink ref="D58" r:id="rId102" xr:uid="{6694919A-D3D6-4B36-A8FE-B5BE69296154}"/>
+    <hyperlink ref="D60" r:id="rId103" xr:uid="{9EBA985F-94C3-43CF-8CF2-69BEB005B4C6}"/>
+    <hyperlink ref="D62" r:id="rId104" xr:uid="{FC477A58-7E10-452F-BED5-FFFF53C282EF}"/>
+    <hyperlink ref="D63" r:id="rId105" xr:uid="{29858BEF-F235-4802-B913-398F6D232B67}"/>
+    <hyperlink ref="D64" r:id="rId106" xr:uid="{97B9AF56-5D25-4703-820F-A71E3BCB0AFE}"/>
+    <hyperlink ref="D65" r:id="rId107" xr:uid="{0A777479-981F-4BA9-B7A4-8450A799351F}"/>
+    <hyperlink ref="D66" r:id="rId108" xr:uid="{86A29DF5-8C10-4E33-AE90-612F7343A0B4}"/>
+    <hyperlink ref="D68" r:id="rId109" xr:uid="{073213B0-822D-4B9C-B2B4-31439DAF1E6B}"/>
+    <hyperlink ref="D69" r:id="rId110" xr:uid="{70591086-16F3-4FF4-AB87-7E6DE7E25C77}"/>
+    <hyperlink ref="D70" r:id="rId111" xr:uid="{C93A29A9-03AC-4796-9E4B-E5310F0D6D93}"/>
+    <hyperlink ref="D72" r:id="rId112" xr:uid="{4B7001EE-74F4-4CA0-86ED-0D3CEFB7A7F4}"/>
+    <hyperlink ref="D80" r:id="rId113" xr:uid="{E4E9DA39-07FB-4241-BB9E-4FD7C86BA8B3}"/>
+    <hyperlink ref="D76" r:id="rId114" xr:uid="{9C26A638-237D-4225-99AA-4D9880AE3063}"/>
+    <hyperlink ref="D74" r:id="rId115" xr:uid="{B82BB00F-FBFB-475B-BBFD-C18C19AEAB28}"/>
+    <hyperlink ref="D77" r:id="rId116" xr:uid="{EEFB76E4-66E2-49A9-92C4-C58EA85F99A9}"/>
+    <hyperlink ref="D78" r:id="rId117" xr:uid="{218F6DC9-BFBE-4C79-8B5B-4A7241E9B331}"/>
+    <hyperlink ref="D83" r:id="rId118" xr:uid="{91DE672F-2AD5-40D4-A1A9-253DDB668FCD}"/>
+    <hyperlink ref="D86" r:id="rId119" xr:uid="{2C1344D1-E099-44CF-A36D-288CFE428D18}"/>
+    <hyperlink ref="D90" r:id="rId120" xr:uid="{F7AD9461-8019-4EB2-840A-576F825C445C}"/>
+    <hyperlink ref="D94" r:id="rId121" xr:uid="{0E8A7917-4F41-4C5D-A0A4-9237B222BC0C}"/>
+    <hyperlink ref="D100" r:id="rId122" xr:uid="{0162D55C-3CB6-4BA3-8FFF-33D68CB44EB8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>